<commit_message>
Login + reporte mejora de timepo
</commit_message>
<xml_diff>
--- a/test_data/test_cases.xlsx
+++ b/test_data/test_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LeandroSouto\qa-dashboard\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961B7EDD-56DE-4C68-B86F-87198A3FA809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA233DE1-44E1-488A-9C07-A96AE98DB83C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{89B8B4F5-96D8-4249-9A59-5A4CFE4348BC}"/>
   </bookViews>
@@ -128,9 +128,6 @@
     <t>FAILED</t>
   </si>
   <si>
-    <t>JIRA-124</t>
-  </si>
-  <si>
     <t>Boton de agregar columna</t>
   </si>
   <si>
@@ -156,6 +153,9 @@
   </si>
   <si>
     <t xml:space="preserve">JIRA-125 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRA-124 </t>
   </si>
 </sst>
 </file>
@@ -579,7 +579,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -694,7 +694,7 @@
         <v>29</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.3">
@@ -702,34 +702,34 @@
         <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>